<commit_message>
Cap nhat 18:35 17/12/2020
</commit_message>
<xml_diff>
--- a/AssyChargeSEHC/bin/Debug/ExcelTemplate.xlsx
+++ b/AssyChargeSEHC/bin/Debug/ExcelTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PM\SEHC\RAV_DuAnSEHC\AssyChargeSEHC\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PM\SEHC\RAV_DuAnSEHC\RAV_DuAnSEHC (16-12-2020)\AssyChargeSEHC\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy\ h:mm:ss"/>
@@ -369,48 +369,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -427,13 +385,1159 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="60">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -996,7 +2100,7 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L1:L1048576"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,14 +2109,14 @@
     <col min="2" max="2" width="21.28515625" style="22" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" style="7" customWidth="1"/>
     <col min="4" max="4" width="13.140625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="38" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="40" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="24" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="26" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" style="11" customWidth="1"/>
     <col min="8" max="8" width="11.85546875" style="15" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" style="9" customWidth="1"/>
     <col min="10" max="10" width="17.28515625" style="9" customWidth="1"/>
     <col min="11" max="11" width="18.42578125" style="9" customWidth="1"/>
-    <col min="12" max="12" width="16.5703125" style="42" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" style="28" customWidth="1"/>
     <col min="13" max="13" width="16.28515625" style="19" customWidth="1"/>
     <col min="14" max="14" width="17.140625" style="20" customWidth="1"/>
     <col min="15" max="15" width="17.85546875" style="20" customWidth="1"/>
@@ -1025,16 +2129,16 @@
       <c r="B1" s="21"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="29" t="s">
+      <c r="E1" s="23"/>
+      <c r="F1" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="31"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="37"/>
       <c r="M1" s="17"/>
       <c r="N1" s="18"/>
       <c r="O1" s="18"/>
@@ -1042,62 +2146,62 @@
       <c r="Q1" s="18"/>
     </row>
     <row r="2" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="32" t="s">
+      <c r="D2" s="39"/>
+      <c r="E2" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="35" t="s">
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="23" t="s">
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="25"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="31"/>
     </row>
     <row r="3" spans="1:17" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="32" t="s">
+      <c r="A3" s="40"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32" t="s">
+      <c r="F3" s="38"/>
+      <c r="G3" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="32"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="28"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="34"/>
     </row>
     <row r="4" spans="1:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="36"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="42"/>
       <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1107,7 +2211,7 @@
       <c r="E4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="F4" s="25" t="s">
         <v>2</v>
       </c>
       <c r="G4" s="3" t="s">
@@ -1125,7 +2229,7 @@
       <c r="K4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="41" t="s">
+      <c r="L4" s="27" t="s">
         <v>11</v>
       </c>
       <c r="M4" s="16" t="s">
@@ -1157,61 +2261,61 @@
     <mergeCell ref="E3:F3"/>
   </mergeCells>
   <conditionalFormatting sqref="L1 L5:L1048576">
-    <cfRule type="cellIs" dxfId="11" priority="20" operator="between">
+    <cfRule type="cellIs" dxfId="23" priority="20" operator="between">
       <formula>24</formula>
-      <formula>25.2</formula>
+      <formula>26</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M5:M1048576">
-    <cfRule type="cellIs" dxfId="10" priority="19" operator="between">
-      <formula>1.45</formula>
+    <cfRule type="cellIs" dxfId="22" priority="19" operator="between">
+      <formula>0.95</formula>
       <formula>1.55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1 Q4:Q1048576">
-    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="13" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5:N1048576">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="notEqual">
-      <formula>"L011X1"</formula>
+    <cfRule type="cellIs" dxfId="20" priority="9" operator="notEqual">
+      <formula>"L0111X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
-      <formula>"L011X1"</formula>
+    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
+      <formula>"L0111X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1 L5:L1048576">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="notBetween">
+    <cfRule type="cellIs" dxfId="18" priority="7" operator="notBetween">
       <formula>24</formula>
-      <formula>25.2</formula>
+      <formula>26</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M3 M5:M1048576">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="notBetween">
-      <formula>1.45</formula>
+    <cfRule type="cellIs" dxfId="17" priority="6" operator="notBetween">
+      <formula>0.95</formula>
       <formula>1.55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q1048576">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O3 O5:O1048576">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="notEqual">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="notEqual">
       <formula>"L111XX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>"L111XX"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P3 P5:P1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="notEqual">
-      <formula>"L0111X"</formula>
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="notEqual">
+      <formula>"L011X1"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>"L0111X"</formula>
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+      <formula>"L011X1"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cap nhat 13:10 22/12/2020
</commit_message>
<xml_diff>
--- a/AssyChargeSEHC/bin/Debug/ExcelTemplate.xlsx
+++ b/AssyChargeSEHC/bin/Debug/ExcelTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Local Disk F_742018351\RAV\SEHC\RAV_DuAnSEHC (22-12-2020)\AssyChargeSEHC\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PM\SEHC\RAV_DuAnSEHC\RAV_DuAnSEHC (22-12-2020)\AssyChargeSEHC\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -78,25 +78,28 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -154,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -162,9 +165,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -174,7 +174,31 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -460,165 +484,163 @@
   <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="W2" sqref="W1:Y1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23.75" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21.375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="20.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="7" customWidth="1"/>
     <col min="5" max="5" width="15" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="15.125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="14.375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="14.875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="16.5" style="2" customWidth="1"/>
-    <col min="11" max="11" width="17.875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="11" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" style="2" customWidth="1"/>
     <col min="12" max="12" width="19" style="2" customWidth="1"/>
     <col min="13" max="13" width="18" style="2" customWidth="1"/>
-    <col min="14" max="14" width="17.25" style="2" customWidth="1"/>
-    <col min="15" max="15" width="18.375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="17.28515625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="18.42578125" style="2" customWidth="1"/>
     <col min="16" max="16" width="18" style="2" customWidth="1"/>
-    <col min="17" max="17" width="15.875" style="2" customWidth="1"/>
-    <col min="18" max="18" width="18.25" style="2" customWidth="1"/>
-    <col min="19" max="19" width="16.125" style="2" customWidth="1"/>
-    <col min="20" max="20" width="15.875" style="2" customWidth="1"/>
-    <col min="21" max="21" width="15.5" style="2" customWidth="1"/>
-    <col min="22" max="22" width="14.625" style="2" customWidth="1"/>
-    <col min="23" max="23" width="15" style="2" customWidth="1"/>
-    <col min="24" max="24" width="16.25" style="2" customWidth="1"/>
-    <col min="25" max="25" width="16.875" style="2" customWidth="1"/>
-    <col min="26" max="26" width="14.875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="15.85546875" style="2" customWidth="1"/>
+    <col min="18" max="18" width="18.28515625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="16.140625" style="11" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" style="11" customWidth="1"/>
+    <col min="21" max="21" width="15.42578125" style="11" customWidth="1"/>
+    <col min="22" max="22" width="14.5703125" style="2" customWidth="1"/>
+    <col min="23" max="23" width="15" style="14" customWidth="1"/>
+    <col min="24" max="24" width="16.28515625" style="14" customWidth="1"/>
+    <col min="25" max="25" width="16.85546875" style="14" customWidth="1"/>
+    <col min="26" max="26" width="14.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="4"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="7" t="s">
+    <row r="1" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7" t="s">
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7" t="s">
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7" t="s">
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7" t="s">
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7" t="s">
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
     </row>
-    <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="R2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="S2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="T2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="U2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="V2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="W2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="X2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Y2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="Z2" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -629,21 +651,19 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
       <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
+      <c r="W3" s="13"/>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="13"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -654,13 +674,13 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
       <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
+      <c r="W4" s="13"/>
+      <c r="X4" s="13"/>
+      <c r="Y4" s="13"/>
       <c r="Z4" s="1"/>
     </row>
   </sheetData>
@@ -673,5 +693,6 @@
     <mergeCell ref="S1:V1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>